<commit_message>
added for those with space
</commit_message>
<xml_diff>
--- a/UpdatedTracker.xlsx
+++ b/UpdatedTracker.xlsx
@@ -1063,9 +1063,21 @@
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1087,9 +1099,21 @@
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1111,9 +1135,21 @@
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
@@ -1135,9 +1171,21 @@
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>

</xml_diff>

<commit_message>
added condition for original date, done today date
</commit_message>
<xml_diff>
--- a/UpdatedTracker.xlsx
+++ b/UpdatedTracker.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -900,7 +903,9 @@
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>type 1 with all files</t>
@@ -919,11 +924,7 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -936,7 +937,9 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>type 2 with missing internal</t>
@@ -960,11 +963,7 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -972,7 +971,9 @@
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
           <t>type 1 with missing outside</t>
@@ -1001,14 +1002,12 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>type 2 with missing number email</t>
@@ -1044,7 +1043,9 @@
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
           <t>type 3 with end date, for type 3 original date=upload date</t>
@@ -1063,16 +1064,8 @@
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1080,7 +1073,9 @@
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
           <t>type 1 with missing internal and outside</t>
@@ -1099,24 +1094,18 @@
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>type 1 with missing internal and number email</t>
@@ -1152,7 +1141,9 @@
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>type 3 with missing outside</t>
@@ -1171,24 +1162,18 @@
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" s="3" t="n">
+        <v>44898</v>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>type 4 with missing internal, outside and number email</t>

</xml_diff>